<commit_message>
📋 TA Scan 2026-02-22 14:55 UTC — 10 nuove posizioni
</commit_message>
<xml_diff>
--- a/output/TA_Monitor_Roma_2026-02-22.xlsx
+++ b/output/TA_Monitor_Roma_2026-02-22.xlsx
@@ -12,7 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Trend 7gg" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nuove Posizioni'!$A$1:$I$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nuove Posizioni'!$A$1:$I$21</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -445,14 +445,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="40" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="45" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="55" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
@@ -506,90 +506,82 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Specialista di Manutenzione / Tecnico di Manutenzione / Manutentore Elettromeccanico / Manutentore Industriale / Manutentore elettrico / Manutentore meccanico, Fiumicino</t>
+          <t>HRBP RETAIL CENTRO ITALIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Amazon.com</t>
+          <t>LHH</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>fulltime</t>
-        </is>
-      </c>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=d5f268ed0d5d0179</t>
+          <t>https://www.linkedin.com/jobs/view/4375811505</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SMART WORKING: Opportunità di Business da Remoto</t>
+          <t>Neolaureato/a con passione per IT e Tecnologia per stage in EgoValeo - Tech Head Hunting (Zona Roma Eur -Rif.1124)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>UDB Team LIA</t>
+          <t>EgoValeo | Tech Head Hunting</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>parttime</t>
-        </is>
-      </c>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=dae1304b2dda199f</t>
+          <t>https://www.linkedin.com/jobs/view/4373152036</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2026-02-22</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Full Stack Developer– AI/GenAI Projects</t>
+          <t>Selezione pubblica, per titoli e colloquio,per n. 2 Tecnologo enti di ricerca liv. III per il CREA DC Sede di Roma</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NTT DATA Europe &amp; Latam</t>
+          <t>Dipartimento della Funzione Pubblica</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -599,7 +591,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
+          <t>Latium, Italy</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -607,24 +599,24 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4314823705</t>
+          <t>https://www.linkedin.com/jobs/view/4373403553</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2026-02-20</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Global Benefits – EMEA Data &amp; Analytics Consulting Lead</t>
+          <t>Responsabile Risorse Umane – Commerciale e Distribuzione</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Aon</t>
+          <t>EmmeBi Group</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -642,104 +634,112 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4367930677</t>
+          <t>https://www.linkedin.com/jobs/view/4374380649</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2026-02-20</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Facility Specialist - Temporary</t>
+          <t>Organico Filiale BARBERINI - Addetti e Addette (FTE)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>myGwork - LGBTQ+ Business Community</t>
+          <t>Globe MKD</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Frosinone, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4373765907</t>
+          <t>https://it.indeed.com/viewjob?jk=a7057852c3f52c5f</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2026-02-21</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cloud Advisory Consultant in ambito IT Strategy</t>
+          <t>Tirocinio Extracurriculare Risorse Umane – Area Gestione del Personale</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>NTT DATA Europe &amp; Latam</t>
+          <t>H501 s.r.l</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>internship</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4340104946</t>
+          <t>https://it.indeed.com/viewjob?jk=211f9c637777d9e6</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Senior Murex Consultant</t>
+          <t>HR Generalist</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NTT DATA Europe &amp; Latam</t>
+          <t>NTWK</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
+          <t>Roma, LAZ, IT</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -747,24 +747,24 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4315869845</t>
+          <t>https://it.indeed.com/viewjob?jk=a202633e80897c25</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Consulente Esperto in Gare d'Appalto e Innovazione IT</t>
+          <t>Buzz Recruitment Day – Lisbon – 09 March 2026</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>NTT DATA Europe &amp; Latam</t>
+          <t>Ryanair - Europe's Favourite Airline</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
+          <t>Fiumicino, Latium, Italy</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -782,24 +782,24 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4334329776</t>
+          <t>https://www.linkedin.com/jobs/view/4374083419</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Operations Supervisor</t>
+          <t>Talent Acquisition Manager</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>myGwork - LGBTQ+ Business Community</t>
+          <t>Jobbit</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -817,24 +817,24 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4373776040</t>
+          <t>https://www.linkedin.com/jobs/view/4375613154</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2026-02-20</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>☕ Recruiting Day | Autogrill: Addetti alla ristorazione - Aeroporto di Roma Fiumicino 🛩️</t>
+          <t>Talent Acquisition &amp; Employer Branding Specialist</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ali Professional</t>
+          <t>Angelini Pharma</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -852,17 +852,343 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" s="2" t="inlineStr">
         <is>
+          <t>https://www.linkedin.com/jobs/view/4375809486</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Specialista di Manutenzione / Tecnico di Manutenzione / Manutentore Elettromeccanico / Manutentore Industriale / Manutentore elettrico / Manutentore meccanico, Fiumicino</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Amazon.com</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=d5f268ed0d5d0179</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SMART WORKING: Opportunità di Business da Remoto</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>UDB Team LIA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>parttime</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=dae1304b2dda199f</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2026-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Full Stack Developer– AI/GenAI Projects</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>NTT DATA Europe &amp; Latam</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4314823705</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Global Benefits – EMEA Data &amp; Analytics Consulting Lead</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Aon</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4367930677</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Facility Specialist - Temporary</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>myGwork - LGBTQ+ Business Community</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Frosinone, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4373765907</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Cloud Advisory Consultant in ambito IT Strategy</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>NTT DATA Europe &amp; Latam</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4340104946</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Senior Murex Consultant</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>NTT DATA Europe &amp; Latam</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4315869845</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Consulente Esperto in Gare d'Appalto e Innovazione IT</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>NTT DATA Europe &amp; Latam</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4334329776</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Operations Supervisor</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>myGwork - LGBTQ+ Business Community</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4373776040</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>☕ Recruiting Day | Autogrill: Addetti alla ristorazione - Aeroporto di Roma Fiumicino 🛩️</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ali Professional</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" s="2" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/jobs/view/4376352851</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I11"/>
+  <autoFilter ref="A1:I21"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -889,7 +1215,7 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Oggi</t>
+          <t>Questa Scan</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
@@ -905,10 +1231,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -918,10 +1244,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -951,7 +1277,7 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Nuove Posizioni</t>
+          <t>Posizioni</t>
         </is>
       </c>
     </row>
@@ -962,7 +1288,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📋 TA Scan 2026-02-22 15:23 UTC — 0 nuove posizioni
</commit_message>
<xml_diff>
--- a/output/TA_Monitor_Roma_2026-02-22.xlsx
+++ b/output/TA_Monitor_Roma_2026-02-22.xlsx
@@ -12,7 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Trend 7gg" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nuove Posizioni'!$A$1:$I$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nuove Posizioni'!$A$1:$I$7</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -541,12 +541,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Neolaureato/a con passione per IT e Tecnologia per stage in EgoValeo - Tech Head Hunting (Zona Roma Eur -Rif.1124)</t>
+          <t>Responsabile Risorse Umane – Commerciale e Distribuzione</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EgoValeo | Tech Head Hunting</t>
+          <t>EmmeBi Group</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -564,34 +564,34 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4373152036</t>
+          <t>https://www.linkedin.com/jobs/view/4374380649</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-20</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Selezione pubblica, per titoli e colloquio,per n. 2 Tecnologo enti di ricerca liv. III per il CREA DC Sede di Roma</t>
+          <t>HR Generalist</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dipartimento della Funzione Pubblica</t>
+          <t>NTWK</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Latium, Italy</t>
+          <t>Roma, LAZ, IT</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -599,24 +599,24 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4373403553</t>
+          <t>https://it.indeed.com/viewjob?jk=a202633e80897c25</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Responsabile Risorse Umane – Commerciale e Distribuzione</t>
+          <t>Buzz Recruitment Day – Lisbon – 09 March 2026</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>EmmeBi Group</t>
+          <t>Ryanair - Europe's Favourite Airline</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
+          <t>Fiumicino, Latium, Italy</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -634,561 +634,87 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4374380649</t>
+          <t>https://www.linkedin.com/jobs/view/4374083419</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Organico Filiale BARBERINI - Addetti e Addette (FTE)</t>
+          <t>Talent Acquisition Manager</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Globe MKD</t>
+          <t>Jobbit</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>fulltime</t>
-        </is>
-      </c>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=a7057852c3f52c5f</t>
+          <t>https://www.linkedin.com/jobs/view/4375613154</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2026-02-21</t>
+          <t>2026-02-20</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tirocinio Extracurriculare Risorse Umane – Area Gestione del Personale</t>
+          <t>Talent Acquisition &amp; Employer Branding Specialist</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>H501 s.r.l</t>
+          <t>Angelini Pharma</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>internship</t>
-        </is>
-      </c>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=211f9c637777d9e6</t>
+          <t>https://www.linkedin.com/jobs/view/4375809486</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>HR Generalist</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>NTWK</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>indeed</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>https://it.indeed.com/viewjob?jk=a202633e80897c25</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2026-02-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Buzz Recruitment Day – Lisbon – 09 March 2026</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Ryanair - Europe's Favourite Airline</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Fiumicino, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4374083419</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>2026-02-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Talent Acquisition Manager</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Jobbit</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4375613154</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
           <t>2026-02-20</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Talent Acquisition &amp; Employer Branding Specialist</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Angelini Pharma</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4375809486</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>2026-02-20</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Specialista di Manutenzione / Tecnico di Manutenzione / Manutentore Elettromeccanico / Manutentore Industriale / Manutentore elettrico / Manutentore meccanico, Fiumicino</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Amazon.com</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>indeed</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>fulltime</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" s="2" t="inlineStr">
-        <is>
-          <t>https://it.indeed.com/viewjob?jk=d5f268ed0d5d0179</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>2026-02-04</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>SMART WORKING: Opportunità di Business da Remoto</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>UDB Team LIA</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>indeed</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>parttime</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" s="2" t="inlineStr">
-        <is>
-          <t>https://it.indeed.com/viewjob?jk=dae1304b2dda199f</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>2026-02-22</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Full Stack Developer– AI/GenAI Projects</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>NTT DATA Europe &amp; Latam</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4314823705</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Global Benefits – EMEA Data &amp; Analytics Consulting Lead</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Aon</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4367930677</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Facility Specialist - Temporary</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>myGwork - LGBTQ+ Business Community</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Frosinone, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4373765907</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Cloud Advisory Consultant in ambito IT Strategy</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>NTT DATA Europe &amp; Latam</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4340104946</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Senior Murex Consultant</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>NTT DATA Europe &amp; Latam</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4315869845</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Consulente Esperto in Gare d'Appalto e Innovazione IT</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>NTT DATA Europe &amp; Latam</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4334329776</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Operations Supervisor</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>myGwork - LGBTQ+ Business Community</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4373776040</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>☕ Recruiting Day | Autogrill: Addetti alla ristorazione - Aeroporto di Roma Fiumicino 🛩️</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Ali Professional</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>linkedin</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4376352851</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I21"/>
+  <autoFilter ref="A1:I7"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1231,10 +757,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -1244,10 +770,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1288,7 +814,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📋 TA Scan 2026-02-22 16:12 UTC — 21 nuove posizioni
</commit_message>
<xml_diff>
--- a/output/TA_Monitor_Roma_2026-02-22.xlsx
+++ b/output/TA_Monitor_Roma_2026-02-22.xlsx
@@ -12,7 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Trend 7gg" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nuove Posizioni'!$A$1:$I$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nuove Posizioni'!$A$1:$I$28</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -506,12 +506,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HRBP RETAIL CENTRO ITALIA</t>
+          <t>Addetto/a Amministrazione del Personale - Ufficio Risorse Umane</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LHH</t>
+          <t>tecno-system</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
+          <t>Fondi, Latium, Italy</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -529,42 +529,46 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4375811505</t>
+          <t>https://www.linkedin.com/jobs/view/4374014717</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Responsabile Risorse Umane – Commerciale e Distribuzione</t>
+          <t>Selezione ROMA CENTRO - Giornate FULL TIME</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EmmeBi Group</t>
+          <t>Globe MKD</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4374380649</t>
+          <t>https://it.indeed.com/viewjob?jk=d58c707c78a09f94</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -576,22 +580,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HR Generalist</t>
+          <t>Impiegato/a Risorse Umane – Servizi alle Imprese</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NTWK</t>
+          <t>tecno-system</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
+          <t>Rome, Latium, Italy</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -599,34 +603,34 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=a202633e80897c25</t>
+          <t>https://www.linkedin.com/jobs/view/4373323755</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-18</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Buzz Recruitment Day – Lisbon – 09 March 2026</t>
+          <t>Procedura di selezione per la chiamata di un professore di prima fascia, GSD 13/ECON-01 - Economia politica, per il Dipartimento di Economics and Financial Markets.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ryanair - Europe's Favourite Airline</t>
+          <t>LIBERA UNIVERSITA' INTERNAZIONALE DEGLI STUDI SOCIALI GUIDO CARLI DI ROMA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Fiumicino, Latium, Italy</t>
+          <t>Roma, LAZ, IT</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -634,24 +638,24 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4374083419</t>
+          <t>https://it.indeed.com/viewjob?jk=4aeb3f7015a7d6ea</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-17</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Talent Acquisition Manager</t>
+          <t>Construction Leadership Academy: Percorso di Alta Formazione e Selezione</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jobbit</t>
+          <t>RADAR - Academy &amp; Recruiting</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -669,24 +673,24 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4375613154</t>
+          <t>https://www.linkedin.com/jobs/view/4374149768</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-17</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Talent Acquisition &amp; Employer Branding Specialist</t>
+          <t>Impiegato/a Risorse Umane</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Angelini Pharma</t>
+          <t>key-absolute</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -704,17 +708,772 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" s="2" t="inlineStr">
         <is>
+          <t>https://www.linkedin.com/jobs/view/4373964211</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Responsabile Risorse Umane – Prodotti per la Cura del Riposo</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>EmmeBi Group</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4374008813</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Recruiter freelance</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Edilizia Alternativa</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4373106227</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>HR ANALYST</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ITA airways</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Fiumicino, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=f8588f663ab8e9fb</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Operatori Recruiting (PART-TIME)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>NTWK</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>parttime</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=cc2eb24c3accfa9c</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Stagista Recruiter</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CONSORZIO STABILE LGA SERVICE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=a82bcd5b613ca42a</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Impiegato/a Ufficio Risorse Umane – Grande Distribuzione Organizzata</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Twins</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=93a5f1a7f8d894c1</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>HR Specialist</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Webgenesys S.p.A.</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=07c6d28d00f459d3</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>HR Business Partner (IT - Remote)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ThinkingIT Corp.</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=5d54341587162f32</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Pilot Recruitment Event in Rome</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Wizz Air</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4373563095</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Graduate Talent Scientist</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Canonical</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4373910412</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>HR Generalist</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Chaberton Professionals</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4371975588</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ADDETTO/A RICERCA E SELEZIONE DEL PERSONALE</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FONDAZIONE LAVORO</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4372870383</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CLIENT RECRUITMENT SPECIALIST ON SITE</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Gi Group</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4372463744</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Talent Acquisition</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>DXC Technology</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4324290308</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>HR Manager (IT - Remote)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ThinkingIT Corp.</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=8435093b0586c1ab</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>HRBP RETAIL CENTRO ITALIA</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>LHH</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4375811505</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Responsabile Risorse Umane – Commerciale e Distribuzione</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>EmmeBi Group</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4374380649</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>HR Generalist</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NTWK</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=a202633e80897c25</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Buzz Recruitment Day – Lisbon – 09 March 2026</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Ryanair - Europe's Favourite Airline</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Fiumicino, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4374083419</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Talent Acquisition Manager</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jobbit</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4375613154</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Talent Acquisition &amp; Employer Branding Specialist</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Angelini Pharma</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" s="2" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/jobs/view/4375809486</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>2026-02-20</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I7"/>
+  <autoFilter ref="A1:I28"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -757,10 +1516,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -770,10 +1529,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -814,7 +1573,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📋 TA Scan 2026-02-22 20:28 UTC — 4 nuove posizioni
</commit_message>
<xml_diff>
--- a/output/TA_Monitor_Roma_2026-02-22.xlsx
+++ b/output/TA_Monitor_Roma_2026-02-22.xlsx
@@ -12,7 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Trend 7gg" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nuove Posizioni'!$A$1:$I$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nuove Posizioni'!$A$1:$I$32</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -506,22 +506,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Addetto/a Amministrazione del Personale - Ufficio Risorse Umane</t>
+          <t>Procedura di selezione per la chiamata di un professore di prima fascia, GSD 14-GSPS-03 - Storia del pensiero e delle istituzioni politiche, per il Dipartimento di scienze politiche.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tecno-system</t>
+          <t>LIBERA UNIVERSITA' INTERNAZIONALE DEGLI STUDI SOCIALI GUIDO CARLI DI ROMA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Fondi, Latium, Italy</t>
+          <t>Roma, LAZ, IT</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -529,46 +529,42 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4374014717</t>
+          <t>https://it.indeed.com/viewjob?jk=81cab064c0c5f569</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Selezione ROMA CENTRO - Giornate FULL TIME</t>
+          <t>Recruiting Marketing Campaign Analyst</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Globe MKD</t>
+          <t>Verisure</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>fulltime</t>
-        </is>
-      </c>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=d58c707c78a09f94</t>
+          <t>https://www.linkedin.com/jobs/view/4373485128</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -580,12 +576,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Impiegato/a Risorse Umane – Servizi alle Imprese</t>
+          <t>Talent Acquisition Specialist</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>tecno-system</t>
+          <t>MioDottore</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -603,34 +599,30 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4373323755</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2026-02-18</t>
-        </is>
-      </c>
+          <t>https://www.linkedin.com/jobs/view/4374991693</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Procedura di selezione per la chiamata di un professore di prima fascia, GSD 13/ECON-01 - Economia politica, per il Dipartimento di Economics and Financial Markets.</t>
+          <t>Buzz Recruitment Day – Rome – 05 March 2026</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LIBERA UNIVERSITA' INTERNAZIONALE DEGLI STUDI SOCIALI GUIDO CARLI DI ROMA</t>
+          <t>Ryanair - Europe's Favourite Airline</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
+          <t>Ciampino, Latium, Italy</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -638,24 +630,24 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=4aeb3f7015a7d6ea</t>
+          <t>https://www.linkedin.com/jobs/view/4374043226</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Construction Leadership Academy: Percorso di Alta Formazione e Selezione</t>
+          <t>Addetto/a Amministrazione del Personale - Ufficio Risorse Umane</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RADAR - Academy &amp; Recruiting</t>
+          <t>tecno-system</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -665,7 +657,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
+          <t>Fondi, Latium, Italy</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -673,59 +665,63 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4374149768</t>
+          <t>https://www.linkedin.com/jobs/view/4374014717</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Impiegato/a Risorse Umane</t>
+          <t>Selezione ROMA CENTRO - Giornate FULL TIME</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>key-absolute</t>
+          <t>Globe MKD</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4373964211</t>
+          <t>https://it.indeed.com/viewjob?jk=d58c707c78a09f94</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-20</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Responsabile Risorse Umane – Prodotti per la Cura del Riposo</t>
+          <t>Impiegato/a Risorse Umane – Servizi alle Imprese</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EmmeBi Group</t>
+          <t>tecno-system</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -743,34 +739,34 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4374008813</t>
+          <t>https://www.linkedin.com/jobs/view/4373323755</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-18</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Recruiter freelance</t>
+          <t>Procedura di selezione per la chiamata di un professore di prima fascia, GSD 13/ECON-01 - Economia politica, per il Dipartimento di Economics and Financial Markets.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Edilizia Alternativa</t>
+          <t>LIBERA UNIVERSITA' INTERNAZIONALE DEGLI STUDI SOCIALI GUIDO CARLI DI ROMA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
+          <t>Roma, LAZ, IT</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -778,34 +774,34 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4373106227</t>
+          <t>https://it.indeed.com/viewjob?jk=4aeb3f7015a7d6ea</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-17</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HR ANALYST</t>
+          <t>Construction Leadership Academy: Percorso di Alta Formazione e Selezione</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ITA airways</t>
+          <t>RADAR - Academy &amp; Recruiting</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Fiumicino, LAZ, IT</t>
+          <t>Rome, Latium, Italy</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -813,141 +809,129 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=f8588f663ab8e9fb</t>
+          <t>https://www.linkedin.com/jobs/view/4374149768</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-17</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Operatori Recruiting (PART-TIME)</t>
+          <t>Impiegato/a Risorse Umane</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>NTWK</t>
+          <t>key-absolute</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>parttime</t>
-        </is>
-      </c>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=cc2eb24c3accfa9c</t>
+          <t>https://www.linkedin.com/jobs/view/4373964211</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2026-02-16</t>
+          <t>2026-02-17</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Stagista Recruiter</t>
+          <t>Responsabile Risorse Umane – Prodotti per la Cura del Riposo</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CONSORZIO STABILE LGA SERVICE</t>
+          <t>EmmeBi Group</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>fulltime</t>
-        </is>
-      </c>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=a82bcd5b613ca42a</t>
+          <t>https://www.linkedin.com/jobs/view/4374008813</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Impiegato/a Ufficio Risorse Umane – Grande Distribuzione Organizzata</t>
+          <t>Recruiter freelance</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Twins</t>
+          <t>Edilizia Alternativa</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>fulltime</t>
-        </is>
-      </c>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=93a5f1a7f8d894c1</t>
+          <t>https://www.linkedin.com/jobs/view/4373106227</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>HR Specialist</t>
+          <t>HR ANALYST</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Webgenesys S.p.A.</t>
+          <t>ITA airways</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -957,7 +941,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
+          <t>Fiumicino, LAZ, IT</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -965,24 +949,24 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=07c6d28d00f459d3</t>
+          <t>https://it.indeed.com/viewjob?jk=f8588f663ab8e9fb</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-01-30</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HR Business Partner (IT - Remote)</t>
+          <t>Operatori Recruiting (PART-TIME)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ThinkingIT Corp.</t>
+          <t>NTWK</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -997,111 +981,119 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>fulltime</t>
+          <t>parttime</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=5d54341587162f32</t>
+          <t>https://it.indeed.com/viewjob?jk=cc2eb24c3accfa9c</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-16</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Pilot Recruitment Event in Rome</t>
+          <t>Stagista Recruiter</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Wizz Air</t>
+          <t>CONSORZIO STABILE LGA SERVICE</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4373563095</t>
+          <t>https://it.indeed.com/viewjob?jk=a82bcd5b613ca42a</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2026-02-16</t>
+          <t>2026-02-17</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Graduate Talent Scientist</t>
+          <t>Impiegato/a Ufficio Risorse Umane – Grande Distribuzione Organizzata</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Canonical</t>
+          <t>Twins</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4373910412</t>
+          <t>https://it.indeed.com/viewjob?jk=93a5f1a7f8d894c1</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-18</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>HR Generalist</t>
+          <t>HR Specialist</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Chaberton Professionals</t>
+          <t>Webgenesys S.p.A.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
+          <t>Roma, LAZ, IT</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -1109,59 +1101,63 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4371975588</t>
+          <t>https://it.indeed.com/viewjob?jk=07c6d28d00f459d3</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-18</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ADDETTO/A RICERCA E SELEZIONE DEL PERSONALE</t>
+          <t>HR Business Partner (IT - Remote)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>FONDAZIONE LAVORO</t>
+          <t>ThinkingIT Corp.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Rome, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4372870383</t>
+          <t>https://it.indeed.com/viewjob?jk=5d54341587162f32</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CLIENT RECRUITMENT SPECIALIST ON SITE</t>
+          <t>Pilot Recruitment Event in Rome</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Gi Group</t>
+          <t>Wizz Air</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1179,24 +1175,24 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4372463744</t>
+          <t>https://www.linkedin.com/jobs/view/4373563095</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-16</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Talent Acquisition</t>
+          <t>Graduate Talent Scientist</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DXC Technology</t>
+          <t>Canonical</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1214,63 +1210,59 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4324290308</t>
+          <t>https://www.linkedin.com/jobs/view/4373910412</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-17</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>HR Manager (IT - Remote)</t>
+          <t>HR Generalist</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ThinkingIT Corp.</t>
+          <t>Chaberton Professionals</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>fulltime</t>
-        </is>
-      </c>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=8435093b0586c1ab</t>
+          <t>https://www.linkedin.com/jobs/view/4371975588</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-17</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>HRBP RETAIL CENTRO ITALIA</t>
+          <t>ADDETTO/A RICERCA E SELEZIONE DEL PERSONALE</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LHH</t>
+          <t>FONDAZIONE LAVORO</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1288,24 +1280,24 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4375811505</t>
+          <t>https://www.linkedin.com/jobs/view/4372870383</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-17</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Responsabile Risorse Umane – Commerciale e Distribuzione</t>
+          <t>CLIENT RECRUITMENT SPECIALIST ON SITE</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>EmmeBi Group</t>
+          <t>Gi Group</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1323,34 +1315,34 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4374380649</t>
+          <t>https://www.linkedin.com/jobs/view/4372463744</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-18</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>HR Generalist</t>
+          <t>Talent Acquisition</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>NTWK</t>
+          <t>DXC Technology</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>indeed</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Roma, LAZ, IT</t>
+          <t>Rome, Latium, Italy</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1358,42 +1350,46 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>https://it.indeed.com/viewjob?jk=a202633e80897c25</t>
+          <t>https://www.linkedin.com/jobs/view/4324290308</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-18</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Buzz Recruitment Day – Lisbon – 09 March 2026</t>
+          <t>HR Manager (IT - Remote)</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Ryanair - Europe's Favourite Airline</t>
+          <t>ThinkingIT Corp.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>linkedin</t>
+          <t>indeed</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Fiumicino, Latium, Italy</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>fulltime</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4374083419</t>
+          <t>https://it.indeed.com/viewjob?jk=8435093b0586c1ab</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1405,12 +1401,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Talent Acquisition Manager</t>
+          <t>HRBP RETAIL CENTRO ITALIA</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Jobbit</t>
+          <t>LHH</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1428,7 +1424,7 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4375613154</t>
+          <t>https://www.linkedin.com/jobs/view/4375811505</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1440,12 +1436,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Talent Acquisition &amp; Employer Branding Specialist</t>
+          <t>Responsabile Risorse Umane – Commerciale e Distribuzione</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Angelini Pharma</t>
+          <t>EmmeBi Group</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1463,17 +1459,157 @@
       <c r="G28" t="inlineStr"/>
       <c r="H28" s="2" t="inlineStr">
         <is>
+          <t>https://www.linkedin.com/jobs/view/4374380649</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>HR Generalist</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>NTWK</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>indeed</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Roma, LAZ, IT</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" s="2" t="inlineStr">
+        <is>
+          <t>https://it.indeed.com/viewjob?jk=a202633e80897c25</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Buzz Recruitment Day – Lisbon – 09 March 2026</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Ryanair - Europe's Favourite Airline</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Fiumicino, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4374083419</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Talent Acquisition Manager</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Jobbit</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" s="2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4375613154</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Talent Acquisition &amp; Employer Branding Specialist</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Angelini Pharma</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Rome, Latium, Italy</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" s="2" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/jobs/view/4375809486</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>2026-02-20</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I28"/>
+  <autoFilter ref="A1:I32"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1516,10 +1652,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -1529,10 +1665,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1573,7 +1709,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>